<commit_message>
Updated results of comparison and model comparings
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/diel-period-habitat/np/glmm_ind_effects_dp_hab_np.xlsx
+++ b/results/accel-glmm-results/diel-period-habitat/np/glmm_ind_effects_dp_hab_np.xlsx
@@ -480,13 +480,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.83634214592032</v>
+        <v>-1.83634214630952</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0334175096121521</v>
+        <v>0.0334175095887593</v>
       </c>
       <c r="G2" t="n">
-        <v>-54.951496004135</v>
+        <v>-54.9514960542485</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -504,16 +504,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>0.319352063026572</v>
+        <v>0.31935206888506</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0618605822130468</v>
+        <v>0.0618605811051425</v>
       </c>
       <c r="G3" t="n">
-        <v>5.16244838961794</v>
+        <v>5.16244857678054</v>
       </c>
       <c r="H3" t="n">
-        <v>0.000000243740588431848</v>
+        <v>0.00000024374034465341</v>
       </c>
     </row>
     <row r="4">
@@ -528,16 +528,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.000674889238349112</v>
+        <v>-0.00067489152186953</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0210441193852176</v>
+        <v>0.0210441193427589</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0320702057422838</v>
+        <v>-0.0320703143180832</v>
       </c>
       <c r="H4" t="n">
-        <v>0.974416063556603</v>
+        <v>0.974415976970188</v>
       </c>
     </row>
     <row r="5">
@@ -552,16 +552,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0348440751122776</v>
+        <v>-0.0348440751986502</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0292886454912161</v>
+        <v>0.0292886453871578</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.1896786118951</v>
+        <v>-1.18967861907086</v>
       </c>
       <c r="H5" t="n">
-        <v>0.234172734903939</v>
+        <v>0.23417273208249</v>
       </c>
     </row>
     <row r="6">
@@ -576,16 +576,16 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0767184693593606</v>
+        <v>0.0767184677251327</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0160294723490567</v>
+        <v>0.0160294722970657</v>
       </c>
       <c r="G6" t="n">
-        <v>4.78608825597902</v>
+        <v>4.78608816955106</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00000170063297196531</v>
+        <v>0.00000170063370391394</v>
       </c>
     </row>
     <row r="7">
@@ -600,16 +600,16 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0161280349941877</v>
+        <v>-0.0161280426113132</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0105496864771963</v>
+        <v>0.0105496864426556</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.52876912778871</v>
+        <v>-1.52876985481792</v>
       </c>
       <c r="H7" t="n">
-        <v>0.126321688272664</v>
+        <v>0.126321507975351</v>
       </c>
     </row>
     <row r="8">
@@ -624,16 +624,16 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0723662726819827</v>
+        <v>0.0723662773576025</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0136430636494986</v>
+        <v>0.013643063532348</v>
       </c>
       <c r="G8" t="n">
-        <v>5.30425383485198</v>
+        <v>5.3042542231091</v>
       </c>
       <c r="H8" t="n">
-        <v>0.000000113134796884168</v>
+        <v>0.000000113134556116697</v>
       </c>
     </row>
     <row r="9">
@@ -648,16 +648,16 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.125641425715419</v>
+        <v>-0.125641422018472</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0104992411660061</v>
+        <v>0.0104992411117505</v>
       </c>
       <c r="G9" t="n">
-        <v>-11.9667149014744</v>
+        <v>-11.9667146111977</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00000000000000000000000000000000530892671694891</v>
+        <v>0.00000000000000000000000000000000530894528541795</v>
       </c>
     </row>
     <row r="10">
@@ -672,16 +672,16 @@
         <v>18</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.128643010972771</v>
+        <v>-0.128643009790711</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0679325116802967</v>
+        <v>0.0679325106220346</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.89368842386087</v>
+        <v>-1.8936884359605</v>
       </c>
       <c r="H10" t="n">
-        <v>0.058266378771921</v>
+        <v>0.0582663771649426</v>
       </c>
     </row>
     <row r="11">
@@ -696,16 +696,16 @@
         <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0159922772704371</v>
+        <v>0.0159922764203322</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0219742590705975</v>
+        <v>0.0219742590580874</v>
       </c>
       <c r="G11" t="n">
-        <v>0.727773219522809</v>
+        <v>0.727773181250743</v>
       </c>
       <c r="H11" t="n">
-        <v>0.466752420667647</v>
+        <v>0.466752444099633</v>
       </c>
     </row>
     <row r="12">
@@ -720,16 +720,16 @@
         <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000368749819157544</v>
+        <v>0.000368749334160286</v>
       </c>
       <c r="F12" t="n">
-        <v>0.030295579524998</v>
+        <v>0.0302955794504742</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0121717367661931</v>
+        <v>0.0121717207872884</v>
       </c>
       <c r="H12" t="n">
-        <v>0.990288598949271</v>
+        <v>0.990288611697648</v>
       </c>
     </row>
     <row r="13">
@@ -744,16 +744,16 @@
         <v>21</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.0359520608542779</v>
+        <v>-0.0359520646812952</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0167818931485291</v>
+        <v>0.0167818931233999</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.14231258273915</v>
+        <v>-2.14231281399148</v>
       </c>
       <c r="H13" t="n">
-        <v>0.032168336981394</v>
+        <v>0.0321683183850265</v>
       </c>
     </row>
     <row r="14">
@@ -768,16 +768,16 @@
         <v>22</v>
       </c>
       <c r="E14" t="n">
-        <v>0.109080740844951</v>
+        <v>0.109080744021057</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0835098376026454</v>
+        <v>0.0835098354282936</v>
       </c>
       <c r="G14" t="n">
-        <v>1.306202286777</v>
+        <v>1.3062023588194</v>
       </c>
       <c r="H14" t="n">
-        <v>0.191483775375979</v>
+        <v>0.19148375088313</v>
       </c>
     </row>
     <row r="15">
@@ -792,16 +792,16 @@
         <v>23</v>
       </c>
       <c r="E15" t="n">
-        <v>0.15166557428827</v>
+        <v>0.151665574520124</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0282536427987634</v>
+        <v>0.0282536426188843</v>
       </c>
       <c r="G15" t="n">
-        <v>5.36800069883053</v>
+        <v>5.36800074121252</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0000000796142452464842</v>
+        <v>0.0000000796142265426834</v>
       </c>
     </row>
     <row r="16">
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0199833042185635</v>
+        <v>0.0199833046549202</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0420906241052281</v>
+        <v>0.0420906237462007</v>
       </c>
       <c r="G16" t="n">
-        <v>0.474768541530877</v>
+        <v>0.474768555947665</v>
       </c>
       <c r="H16" t="n">
-        <v>0.634951957788889</v>
+        <v>0.634951947511982</v>
       </c>
     </row>
     <row r="17">
@@ -840,16 +840,16 @@
         <v>25</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.0537789261659025</v>
+        <v>-0.0537789278321617</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0223246569688788</v>
+        <v>0.0223246568251166</v>
       </c>
       <c r="G17" t="n">
-        <v>-2.4089474808447</v>
+        <v>-2.408947570995</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0159986000498454</v>
+        <v>0.0159985960980388</v>
       </c>
     </row>
     <row r="18">
@@ -864,16 +864,16 @@
         <v>26</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.0561918667824113</v>
+        <v>-0.0561918651256012</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0647769168560062</v>
+        <v>0.0647769156424572</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.867467448432615</v>
+        <v>-0.867467439106827</v>
       </c>
       <c r="H18" t="n">
-        <v>0.385685939778985</v>
+        <v>0.38568594488665</v>
       </c>
     </row>
     <row r="19">
@@ -888,16 +888,16 @@
         <v>27</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.00150425397945481</v>
+        <v>-0.00150425382705733</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0219787114096313</v>
+        <v>0.0219787113513368</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.0684414091171712</v>
+        <v>-0.0684414023648314</v>
       </c>
       <c r="H19" t="n">
-        <v>0.94543425938205</v>
+        <v>0.945434264757035</v>
       </c>
     </row>
     <row r="20">
@@ -912,16 +912,16 @@
         <v>28</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0343595487786216</v>
+        <v>0.0343595488636084</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0309234187645534</v>
+        <v>0.030923418625161</v>
       </c>
       <c r="G20" t="n">
-        <v>1.11111740394005</v>
+        <v>1.11111741169689</v>
       </c>
       <c r="H20" t="n">
-        <v>0.266517817475787</v>
+        <v>0.266517814137383</v>
       </c>
     </row>
     <row r="21">
@@ -936,16 +936,16 @@
         <v>29</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0135510023287434</v>
+        <v>-0.0135510006317084</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0167194075004251</v>
+        <v>0.0167194074327267</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.810495367637807</v>
+        <v>-0.810495269418677</v>
       </c>
       <c r="H21" t="n">
-        <v>0.417655526362766</v>
+        <v>0.417655582790361</v>
       </c>
     </row>
     <row r="22">
@@ -962,7 +962,7 @@
         <v>32</v>
       </c>
       <c r="E22" t="n">
-        <v>0.141633181922872</v>
+        <v>0.141633181925008</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>

</xml_diff>